<commit_message>
add session for debugging bug #98
</commit_message>
<xml_diff>
--- a/Sessions/ABC/ABC_Acceptance_Criteria_NoDose.xlsx
+++ b/Sessions/ABC/ABC_Acceptance_Criteria_NoDose.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="122211" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -167,23 +167,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -219,23 +202,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -415,12 +381,12 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -437,7 +403,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -448,13 +414,13 @@
         <v>2</v>
       </c>
       <c r="D2">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>0.15</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -465,13 +431,13 @@
         <v>3</v>
       </c>
       <c r="D3">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>0.35</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -482,13 +448,13 @@
         <v>2</v>
       </c>
       <c r="D4">
-        <v>0.45</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>0.55000000000000004</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -499,10 +465,10 @@
         <v>3</v>
       </c>
       <c r="D5">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>0.4</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -519,9 +485,9 @@
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>2</v>
       </c>
@@ -543,7 +509,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>